<commit_message>
Reformatted and fixed all of the sprint backlogs.
</commit_message>
<xml_diff>
--- a/Deliverable_2/Blackbear-Consultants_Deliverable_2_SprintBacklog_2.xlsx
+++ b/Deliverable_2/Blackbear-Consultants_Deliverable_2_SprintBacklog_2.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Blackbear-Consultants-Git/Deliverable_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdullahkarim/Documents/GitHub/Blackbear-Consultants/Deliverable_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C8F4E33-5873-AF43-86D2-DEB55762FC80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED0A6C6-9DC8-D04E-97D6-E5448B2B653E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18400" windowHeight="12580" activeTab="1" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="3" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
+    <sheet name="D1-Sprint 1" sheetId="3" r:id="rId1"/>
+    <sheet name="D1-Sprint 2" sheetId="4" r:id="rId2"/>
+    <sheet name="D2-Sprint 3" sheetId="1" r:id="rId3"/>
+    <sheet name="D2-Sprint 4" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="24">
   <si>
     <t>Sprint Goal</t>
   </si>
@@ -245,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
@@ -300,6 +302,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +620,506 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488A9DCE-42DD-074C-B76C-FB872E3590EF}">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="59.83203125" customWidth="1"/>
+    <col min="2" max="2" width="95.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="9.33203125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="M8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="24"/>
+    </row>
+    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="M9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="M10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="M11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+    </row>
+    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+    </row>
+    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34419BF5-2540-6C49-ADAF-DDB784C8E83A}">
+  <dimension ref="A1:S15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="59.83203125" customWidth="1"/>
+    <col min="2" max="2" width="95.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="9.33203125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="M8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="24"/>
+    </row>
+    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="M9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="M10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="M11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+    </row>
+    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+    </row>
+    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC36FCF-9F37-4AC5-B7F3-1DC0EDBEC864}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -863,7 +1365,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E3A477-5022-4EBF-A5F0-EFD4BBDA3FE6}">
   <dimension ref="A1:N12"/>
   <sheetViews>

</xml_diff>